<commit_message>
Some filtering steps possibly weren't saved
Saved again, and pushed the updated file.
</commit_message>
<xml_diff>
--- a/Data/Adgangskvotienter - videregående uddannelser - updated.xlsx
+++ b/Data/Adgangskvotienter - videregående uddannelser - updated.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\whart\OneDrive\Skrivebord\Uni\9. semester\Data visualization\Group Project\datavis\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3609B017-3EE0-41BE-B084-735CC93624E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2404749C-C804-4C01-89AF-D43DC736934E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{1F6E294E-15E8-45DD-9837-2A0AD2A2219D}"/>
   </bookViews>
@@ -2891,7 +2891,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>